<commit_message>
feat: refactored pathway and swr analysis pipeline
</commit_message>
<xml_diff>
--- a/gym/analysis/cook_disordered/sorted/info/info.xlsx
+++ b/gym/analysis/cook_disordered/sorted/info/info.xlsx
@@ -366,63 +366,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>-80969.84687153777</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-93493.83739772075</v>
       </c>
-      <c r="D2">
-        <v>-106017.4941373419</v>
+      <c r="E2">
+        <v>-106017.1405710956</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>-80969.5736773855</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-93493.80312253101</v>
       </c>
-      <c r="D3">
-        <v>-106017.1405710956</v>
+      <c r="E3">
+        <v>-106016.8796549928</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>-80969.33619137455</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-93493.46436009509</v>
-      </c>
-      <c r="D4">
-        <v>-106016.8796549928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>